<commit_message>
forgot to plot the last
</commit_message>
<xml_diff>
--- a/10g/test12345.xlsx
+++ b/10g/test12345.xlsx
@@ -230,24 +230,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63408000"/>
-        <c:axId val="63409536"/>
+        <c:axId val="123682176"/>
+        <c:axId val="125863040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63408000"/>
+        <c:axId val="123682176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63409536"/>
+        <c:crossAx val="125863040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63409536"/>
+        <c:axId val="125863040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -255,7 +255,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63408000"/>
+        <c:crossAx val="123682176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -268,7 +268,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -433,24 +433,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64775296"/>
-        <c:axId val="64844160"/>
+        <c:axId val="125891712"/>
+        <c:axId val="125893248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64775296"/>
+        <c:axId val="125891712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64844160"/>
+        <c:crossAx val="125893248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64844160"/>
+        <c:axId val="125893248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +458,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64775296"/>
+        <c:crossAx val="125891712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -471,7 +471,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -636,24 +636,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118337920"/>
-        <c:axId val="118339840"/>
+        <c:axId val="156715648"/>
+        <c:axId val="156725632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118337920"/>
+        <c:axId val="156715648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118339840"/>
+        <c:crossAx val="156725632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118339840"/>
+        <c:axId val="156725632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +661,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118337920"/>
+        <c:crossAx val="156715648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -674,7 +674,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -839,24 +839,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="137344512"/>
-        <c:axId val="137346048"/>
+        <c:axId val="156746112"/>
+        <c:axId val="156747648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137344512"/>
+        <c:axId val="156746112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137346048"/>
+        <c:crossAx val="156747648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137346048"/>
+        <c:axId val="156747648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +864,210 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137344512"/>
+        <c:crossAx val="156746112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fo-FO"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Moose</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$B$86:$Q$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wolf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$B$87:$Q$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="168857984"/>
+        <c:axId val="168859520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="168857984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="168859520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="168859520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="168857984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,6 +1203,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagram 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1295,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="R73" sqref="R73"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>